<commit_message>
Add budget item exceptions including ui and db access.
</commit_message>
<xml_diff>
--- a/TestBudget.xlsx
+++ b/TestBudget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PersonalMyCode\BudgetUpdator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E059BD1F-0ECC-4656-B348-A5C084B88084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F24B8B-D937-4730-BE05-C5D2EAE2A855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="0" windowWidth="28770" windowHeight="15465" activeTab="1" xr2:uid="{AF956A61-A15A-4A6E-9A9E-CFD1D374AF1F}"/>
+    <workbookView xWindow="-23595" yWindow="1890" windowWidth="22755" windowHeight="10125" activeTab="1" xr2:uid="{AF956A61-A15A-4A6E-9A9E-CFD1D374AF1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Income" sheetId="2" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
   <si>
     <t>May</t>
   </si>
@@ -126,9 +126,15 @@
     <t>Walmart</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>Rewards</t>
   </si>
   <si>
+    <t>Groceries</t>
+  </si>
+  <si>
     <t>Checking</t>
   </si>
   <si>
@@ -147,9 +153,6 @@
     <t>Citi</t>
   </si>
   <si>
-    <t>Groceries</t>
-  </si>
-  <si>
     <t>Venmo</t>
   </si>
   <si>
@@ -415,6 +418,9 @@
   </si>
   <si>
     <t>Xfinity Mobile</t>
+  </si>
+  <si>
+    <t>Newpark Resort Park City Ut Visa</t>
   </si>
   <si>
     <t>123</t>
@@ -1200,8 +1206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46617975-4435-450D-8E4F-CA1A567C5B3E}">
   <dimension ref="A1:AR200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L23" workbookViewId="0">
-      <selection activeCell="AC44" sqref="AC44"/>
+    <sheetView tabSelected="1" topLeftCell="L5" workbookViewId="0">
+      <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,7 +1382,7 @@
       <c r="X6" s="26"/>
       <c r="Y6" s="25">
         <f>SUM(Y8:Y199)</f>
-        <v>809.3600000000002</v>
+        <v>517.6299999999999</v>
       </c>
       <c r="Z6" s="26"/>
       <c r="AA6" s="27"/>
@@ -1493,11 +1499,15 @@
       <c r="U8" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="V8" s="47"/>
+      <c r="V8" s="47" t="s">
+        <v>21</v>
+      </c>
       <c r="W8" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="X8" s="47"/>
+        <v>22</v>
+      </c>
+      <c r="X8" s="47" t="s">
+        <v>23</v>
+      </c>
       <c r="Y8" s="48">
         <v>17.14</v>
       </c>
@@ -1507,10 +1517,10 @@
       <c r="AI8" s="14"/>
       <c r="AJ8" s="14"/>
       <c r="AK8" s="49" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="AM8" s="50" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AN8" s="51" t="str">
         <f>VLOOKUP(AN7,AN11:AO22,2,FALSE)</f>
@@ -1520,7 +1530,7 @@
     <row r="9" ht="15.75">
       <c r="B9" s="40"/>
       <c r="C9" s="40" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D9" s="52" cm="1">
         <f ref="D9:D9" t="array" aca="1" ca="1">INDIRECT("Income!"&amp;AN8)</f>
@@ -1529,7 +1539,7 @@
       <c r="E9" s="40"/>
       <c r="G9" s="41"/>
       <c r="H9" s="53" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I9" s="42"/>
       <c r="J9" s="54"/>
@@ -1547,10 +1557,10 @@
         <v>45438</v>
       </c>
       <c r="U9" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="W9" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y9" s="70">
         <v>10.69</v>
@@ -1561,7 +1571,7 @@
       <c r="AI9" s="14"/>
       <c r="AJ9" s="14"/>
       <c r="AK9" s="49" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10">
@@ -1576,7 +1586,7 @@
       <c r="E10" s="40"/>
       <c r="G10" s="41"/>
       <c r="H10" s="56" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I10" s="10" t="e" cm="1">
         <f ref="I10:I10" t="array" aca="1" ca="1">INDIRECT($AN$7&amp;"!"&amp;"O10")</f>
@@ -1608,10 +1618,10 @@
         <v>45438</v>
       </c>
       <c r="U10" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="W10" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y10" s="70">
         <v>50.73</v>
@@ -1622,31 +1632,31 @@
       <c r="AI10" s="14"/>
       <c r="AJ10" s="14"/>
       <c r="AK10" s="49" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AM10" s="50" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AN10" s="50" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AO10" s="50" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="40"/>
       <c r="C11" s="40" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11" s="58">
         <f>Y6</f>
-        <v>809.3600000000002</v>
+        <v>517.6299999999999</v>
       </c>
       <c r="E11" s="40"/>
       <c r="G11" s="41"/>
       <c r="H11" s="56" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I11" s="10" t="e" cm="1">
         <f ref="I11:I11" t="array" aca="1" ca="1">INDIRECT($AN$7&amp;"!"&amp;"O11")</f>
@@ -1668,7 +1678,7 @@
         <v>#REF!</v>
       </c>
       <c r="N11" s="57" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O11" s="10" t="e">
         <f>IF(N11="y",M11,)</f>
@@ -1683,10 +1693,10 @@
         <v>45438</v>
       </c>
       <c r="U11" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="W11" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y11" s="70">
         <v>264.03</v>
@@ -1697,16 +1707,16 @@
       <c r="AI11" s="14"/>
       <c r="AJ11" s="14"/>
       <c r="AK11" s="49" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AM11" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AN11" s="59" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AO11" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AR11" s="28"/>
     </row>
@@ -1717,7 +1727,7 @@
       <c r="E12" s="40"/>
       <c r="G12" s="41"/>
       <c r="H12" s="56" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I12" s="10" t="e" cm="1">
         <f ref="I12:I12" t="array" aca="1" ca="1">INDIRECT($AN$7&amp;"!"&amp;"O12")</f>
@@ -1739,7 +1749,7 @@
         <v>#REF!</v>
       </c>
       <c r="N12" s="57" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O12" s="10" t="e">
         <f ref="O12:O21" t="shared" si="3" ca="1">IF(N12="y",M12,)</f>
@@ -1754,10 +1764,10 @@
         <v>45437</v>
       </c>
       <c r="U12" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="W12" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y12" s="70">
         <v>24.34</v>
@@ -1768,30 +1778,30 @@
       <c r="AI12" s="14"/>
       <c r="AJ12" s="14"/>
       <c r="AK12" s="49" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AM12" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AN12" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AO12" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="14"/>
       <c r="B13" s="40"/>
       <c r="C13" s="40" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D13" s="40"/>
       <c r="E13" s="40"/>
       <c r="F13" s="14"/>
       <c r="G13" s="41"/>
       <c r="H13" s="56" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I13" s="10" t="e" cm="1">
         <f ref="I13:I13" t="array" aca="1" ca="1">INDIRECT($AN$7&amp;"!"&amp;"O13")</f>
@@ -1813,7 +1823,7 @@
         <v>#REF!</v>
       </c>
       <c r="N13" s="57" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O13" s="10" t="e">
         <f t="shared" si="3" ca="1"/>
@@ -1830,8 +1840,14 @@
       <c r="U13" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="V13" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W13" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="X13" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="Y13" s="70">
         <v>150.7</v>
@@ -1842,23 +1858,23 @@
       <c r="AI13" s="14"/>
       <c r="AJ13" s="14"/>
       <c r="AK13" s="49" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AM13" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AN13" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AO13" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="14"/>
       <c r="B14" s="61"/>
       <c r="C14" s="62" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D14" s="48">
         <v>-454.02</v>
@@ -1867,7 +1883,7 @@
       <c r="F14" s="14"/>
       <c r="G14" s="41"/>
       <c r="H14" s="56" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I14" s="10" t="e" cm="1">
         <f ref="I14:I14" t="array" aca="1" ca="1">INDIRECT($AN$7&amp;"!"&amp;"O14")</f>
@@ -1889,7 +1905,7 @@
         <v>#REF!</v>
       </c>
       <c r="N14" s="57" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O14" s="10" t="e">
         <f t="shared" si="3" ca="1"/>
@@ -1906,8 +1922,14 @@
       <c r="U14" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="V14" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W14" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="X14" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="Y14" s="70">
         <v>140.8</v>
@@ -1918,33 +1940,33 @@
       <c r="AI14" s="14"/>
       <c r="AJ14" s="14"/>
       <c r="AK14" s="49" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AM14" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AN14" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AO14" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="14"/>
       <c r="B15" s="61"/>
       <c r="C15" s="40" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D15" s="60">
         <f>D9-D11</f>
-        <v>-809.3600000000002</v>
+        <v>-517.6299999999999</v>
       </c>
       <c r="E15" s="61"/>
       <c r="F15" s="14"/>
       <c r="G15" s="41"/>
       <c r="H15" s="56" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I15" s="10" t="e" cm="1">
         <f ref="I15:I15" t="array" aca="1" ca="1">INDIRECT($AN$7&amp;"!"&amp;"O15")</f>
@@ -1966,7 +1988,7 @@
         <v>#REF!</v>
       </c>
       <c r="N15" s="57" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O15" s="10" t="e">
         <f t="shared" si="3" ca="1"/>
@@ -1981,10 +2003,10 @@
         <v>45434</v>
       </c>
       <c r="U15" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="W15" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y15" s="70">
         <v>66.3</v>
@@ -1998,10 +2020,10 @@
         <v>0</v>
       </c>
       <c r="AN15" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AO15" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AR15" s="28"/>
     </row>
@@ -2014,7 +2036,7 @@
       <c r="F16" s="14"/>
       <c r="G16" s="41"/>
       <c r="H16" s="56" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I16" s="10" t="e" cm="1">
         <f ref="I16:I16" t="array" aca="1" ca="1">INDIRECT($AN$7&amp;"!"&amp;"O16")</f>
@@ -2049,10 +2071,10 @@
         <v>45434</v>
       </c>
       <c r="U16" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="W16" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y16" s="70">
         <v>8.53</v>
@@ -2063,13 +2085,13 @@
       <c r="AI16" s="14"/>
       <c r="AJ16" s="14"/>
       <c r="AM16" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AN16" s="0" t="s">
         <v>0</v>
       </c>
       <c r="AO16" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17">
@@ -2081,7 +2103,7 @@
       <c r="F17" s="14"/>
       <c r="G17" s="41"/>
       <c r="H17" s="56" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I17" s="10" t="e" cm="1">
         <f ref="I17:I17" t="array" aca="1" ca="1">INDIRECT($AN$7&amp;"!"&amp;"O17")</f>
@@ -2103,7 +2125,7 @@
         <v>#REF!</v>
       </c>
       <c r="N17" s="57" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O17" s="10" t="e">
         <f t="shared" si="3" ca="1"/>
@@ -2118,10 +2140,10 @@
         <v>45433</v>
       </c>
       <c r="U17" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="W17" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y17" s="70">
         <v>47.45</v>
@@ -2132,13 +2154,13 @@
       <c r="AI17" s="14"/>
       <c r="AJ17" s="14"/>
       <c r="AM17" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AN17" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AO17" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18">
@@ -2183,8 +2205,14 @@
       <c r="U18" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="V18" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W18" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="X18" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="Y18" s="70">
         <v>58.51</v>
@@ -2195,13 +2223,13 @@
       <c r="AI18" s="14"/>
       <c r="AJ18" s="14"/>
       <c r="AM18" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AN18" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AO18" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19">
@@ -2244,10 +2272,10 @@
         <v>45431</v>
       </c>
       <c r="U19" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="W19" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y19" s="70">
         <v>-2046.1</v>
@@ -2258,13 +2286,13 @@
       <c r="AI19" s="14"/>
       <c r="AJ19" s="14"/>
       <c r="AM19" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AN19" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AO19" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AR19" s="28"/>
     </row>
@@ -2310,8 +2338,14 @@
       <c r="U20" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="V20" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W20" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="X20" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="Y20" s="70">
         <v>5.51</v>
@@ -2322,13 +2356,13 @@
       <c r="AI20" s="14"/>
       <c r="AJ20" s="14"/>
       <c r="AM20" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AN20" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AO20" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21">
@@ -2371,10 +2405,10 @@
         <v>45430</v>
       </c>
       <c r="U21" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="W21" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y21" s="70">
         <v>29.07</v>
@@ -2385,13 +2419,13 @@
       <c r="AI21" s="14"/>
       <c r="AJ21" s="14"/>
       <c r="AM21" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AN21" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AO21" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AP21" s="66"/>
     </row>
@@ -2404,7 +2438,7 @@
       <c r="F22" s="14"/>
       <c r="G22" s="41"/>
       <c r="H22" s="67" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I22" s="42"/>
       <c r="J22" s="54"/>
@@ -2425,10 +2459,10 @@
         <v>45429</v>
       </c>
       <c r="U22" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="W22" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y22" s="70">
         <v>133.9</v>
@@ -2439,13 +2473,13 @@
       <c r="AI22" s="14"/>
       <c r="AJ22" s="14"/>
       <c r="AM22" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AN22" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AO22" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AP22" s="66"/>
     </row>
@@ -2458,7 +2492,7 @@
       <c r="F23" s="14"/>
       <c r="G23" s="41"/>
       <c r="H23" s="56" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I23" s="42"/>
       <c r="J23" s="54">
@@ -2487,10 +2521,10 @@
         <v>45429</v>
       </c>
       <c r="U23" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="W23" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y23" s="70">
         <v>60.61</v>
@@ -2511,7 +2545,7 @@
       <c r="F24" s="14"/>
       <c r="G24" s="41"/>
       <c r="H24" s="56" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I24" s="42"/>
       <c r="J24" s="54">
@@ -2540,10 +2574,10 @@
         <v>45429</v>
       </c>
       <c r="U24" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="W24" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y24" s="70">
         <v>21.67</v>
@@ -2563,7 +2597,7 @@
       <c r="F25" s="14"/>
       <c r="G25" s="41"/>
       <c r="H25" s="56" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I25" s="42"/>
       <c r="J25" s="54">
@@ -2592,10 +2626,10 @@
         <v>45428</v>
       </c>
       <c r="U25" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="W25" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y25" s="70">
         <v>76.67</v>
@@ -2615,7 +2649,7 @@
       <c r="F26" s="14"/>
       <c r="G26" s="41"/>
       <c r="H26" s="56" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I26" s="42"/>
       <c r="J26" s="54">
@@ -2644,10 +2678,10 @@
         <v>45428</v>
       </c>
       <c r="U26" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W26" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y26" s="70">
         <v>59.95</v>
@@ -2667,7 +2701,7 @@
       <c r="F27" s="14"/>
       <c r="G27" s="41"/>
       <c r="H27" s="56" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I27" s="42"/>
       <c r="J27" s="54">
@@ -2696,10 +2730,10 @@
         <v>45428</v>
       </c>
       <c r="U27" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="W27" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y27" s="70">
         <v>13.73</v>
@@ -2720,7 +2754,7 @@
       <c r="F28" s="14"/>
       <c r="G28" s="41"/>
       <c r="H28" s="56" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I28" s="42"/>
       <c r="J28" s="54">
@@ -2749,10 +2783,10 @@
         <v>45427</v>
       </c>
       <c r="U28" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="W28" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y28" s="70">
         <v>95.58</v>
@@ -2772,7 +2806,7 @@
       <c r="F29" s="14"/>
       <c r="G29" s="41"/>
       <c r="H29" s="56" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I29" s="42"/>
       <c r="J29" s="54">
@@ -2801,10 +2835,10 @@
         <v>45426</v>
       </c>
       <c r="U29" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="W29" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y29" s="70">
         <v>3.22</v>
@@ -2824,7 +2858,7 @@
       <c r="F30" s="14"/>
       <c r="G30" s="41"/>
       <c r="H30" s="56" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I30" s="42"/>
       <c r="J30" s="54">
@@ -2853,10 +2887,10 @@
         <v>45425</v>
       </c>
       <c r="U30" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="W30" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y30" s="70">
         <v>86.38</v>
@@ -2876,7 +2910,7 @@
       <c r="F31" s="14"/>
       <c r="G31" s="41"/>
       <c r="H31" s="56" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I31" s="42"/>
       <c r="J31" s="54">
@@ -2907,8 +2941,14 @@
       <c r="U31" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="V31" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W31" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="X31" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="Y31" s="70">
         <v>158.27</v>
@@ -2954,10 +2994,10 @@
         <v>45424</v>
       </c>
       <c r="U32" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="W32" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y32" s="70">
         <v>7.48</v>
@@ -3002,10 +3042,10 @@
         <v>45422</v>
       </c>
       <c r="U33" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="W33" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y33" s="70">
         <v>14.35</v>
@@ -3043,8 +3083,14 @@
       <c r="U34" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="V34" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W34" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="X34" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="Y34" s="70">
         <v>180.94</v>
@@ -3091,8 +3137,14 @@
       <c r="U35" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="V35" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W35" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="X35" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="Y35" s="70">
         <v>4.73</v>
@@ -3138,10 +3190,10 @@
         <v>45421</v>
       </c>
       <c r="U36" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="W36" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y36" s="70">
         <v>32.22</v>
@@ -3177,10 +3229,10 @@
         <v>45421</v>
       </c>
       <c r="U37" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="W37" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y37" s="70">
         <v>780.78</v>
@@ -3200,7 +3252,7 @@
       <c r="F38" s="14"/>
       <c r="G38" s="41"/>
       <c r="H38" s="67" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I38" s="42"/>
       <c r="J38" s="54"/>
@@ -3227,10 +3279,10 @@
         <v>45421</v>
       </c>
       <c r="U38" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="W38" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y38" s="70">
         <v>-3.42</v>
@@ -3250,7 +3302,7 @@
       <c r="F39" s="14"/>
       <c r="G39" s="41"/>
       <c r="H39" s="56" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I39" s="42"/>
       <c r="J39" s="54">
@@ -3279,10 +3331,10 @@
         <v>45421</v>
       </c>
       <c r="U39" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="W39" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y39" s="70">
         <v>26</v>
@@ -3303,7 +3355,7 @@
       <c r="F40" s="14"/>
       <c r="G40" s="41"/>
       <c r="H40" s="56" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I40" s="42"/>
       <c r="J40" s="54">
@@ -3332,10 +3384,10 @@
         <v>45420</v>
       </c>
       <c r="U40" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="W40" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y40" s="70">
         <v>18.53</v>
@@ -3355,7 +3407,7 @@
       <c r="F41" s="14"/>
       <c r="G41" s="41"/>
       <c r="H41" s="56" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I41" s="42"/>
       <c r="J41" s="54">
@@ -3384,10 +3436,10 @@
         <v>45420</v>
       </c>
       <c r="U41" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="W41" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y41" s="70">
         <v>27.45</v>
@@ -3407,7 +3459,7 @@
       <c r="F42" s="14"/>
       <c r="G42" s="41"/>
       <c r="H42" s="56" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I42" s="42"/>
       <c r="J42" s="54">
@@ -3436,10 +3488,10 @@
         <v>45420</v>
       </c>
       <c r="U42" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="W42" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y42" s="70">
         <v>12.84</v>
@@ -3459,7 +3511,7 @@
       <c r="F43" s="14"/>
       <c r="G43" s="41"/>
       <c r="H43" s="56" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I43" s="42"/>
       <c r="J43" s="54">
@@ -3488,10 +3540,10 @@
         <v>45419</v>
       </c>
       <c r="U43" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="W43" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y43" s="70">
         <v>69.56</v>
@@ -3512,7 +3564,7 @@
       <c r="F44" s="14"/>
       <c r="G44" s="41"/>
       <c r="H44" s="56" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I44" s="42"/>
       <c r="J44" s="54">
@@ -3541,10 +3593,10 @@
         <v>45417</v>
       </c>
       <c r="U44" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="W44" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y44" s="70">
         <v>21.76</v>
@@ -3589,10 +3641,10 @@
         <v>45417</v>
       </c>
       <c r="U45" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="W45" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y45" s="70">
         <v>3.22</v>
@@ -3637,10 +3689,10 @@
         <v>45417</v>
       </c>
       <c r="U46" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="W46" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y46" s="70">
         <v>58</v>
@@ -3685,10 +3737,10 @@
         <v>45417</v>
       </c>
       <c r="U47" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="W47" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y47" s="70">
         <v>47.1</v>
@@ -3734,10 +3786,10 @@
         <v>45417</v>
       </c>
       <c r="U48" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="W48" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y48" s="70">
         <v>-1647.72</v>
@@ -3782,10 +3834,10 @@
         <v>45416</v>
       </c>
       <c r="U49" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="W49" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y49" s="70">
         <v>10.35</v>
@@ -3830,10 +3882,10 @@
         <v>45416</v>
       </c>
       <c r="U50" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="W50" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y50" s="70">
         <v>17.11</v>
@@ -3878,10 +3930,10 @@
         <v>45416</v>
       </c>
       <c r="U51" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="W51" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y51" s="70">
         <v>904.99</v>
@@ -3926,10 +3978,10 @@
         <v>45415</v>
       </c>
       <c r="U52" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="W52" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y52" s="70">
         <v>24.71</v>
@@ -3976,8 +4028,14 @@
       <c r="U53" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="V53" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W53" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="X53" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="Y53" s="70">
         <v>48.18</v>
@@ -4022,11 +4080,11 @@
         <v>45415</v>
       </c>
       <c r="U54" s="47" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="V54" s="47"/>
       <c r="W54" s="47" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X54" s="47"/>
       <c r="Y54" s="48">
@@ -4072,11 +4130,11 @@
         <v>45414</v>
       </c>
       <c r="U55" s="47" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="V55" s="47"/>
       <c r="W55" s="47" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X55" s="47"/>
       <c r="Y55" s="48">
@@ -4122,11 +4180,11 @@
         <v>45414</v>
       </c>
       <c r="U56" s="47" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="V56" s="47"/>
       <c r="W56" s="47" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X56" s="47"/>
       <c r="Y56" s="48">
@@ -4172,11 +4230,11 @@
         <v>45414</v>
       </c>
       <c r="U57" s="47" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="V57" s="47"/>
       <c r="W57" s="47" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X57" s="47"/>
       <c r="Y57" s="48">
@@ -4222,11 +4280,11 @@
         <v>45413</v>
       </c>
       <c r="U58" s="47" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="V58" s="47"/>
       <c r="W58" s="47" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X58" s="47"/>
       <c r="Y58" s="48">
@@ -4263,11 +4321,11 @@
         <v>45413</v>
       </c>
       <c r="U59" s="47" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="V59" s="47"/>
       <c r="W59" s="47" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X59" s="47"/>
       <c r="Y59" s="48">
@@ -4298,21 +4356,21 @@
       <c r="P60" s="1"/>
       <c r="R60" s="45"/>
       <c r="S60" s="45">
-        <v>1596</v>
+        <v>116</v>
       </c>
       <c r="T60" s="46">
-        <v>45438</v>
+        <v>45441</v>
       </c>
       <c r="U60" s="47" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="V60" s="47"/>
       <c r="W60" s="47" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X60" s="47"/>
       <c r="Y60" s="48">
-        <v>264.03</v>
+        <v>10.69</v>
       </c>
       <c r="Z60" s="45"/>
       <c r="AA60" s="14"/>
@@ -4339,21 +4397,21 @@
       <c r="P61" s="1"/>
       <c r="R61" s="45"/>
       <c r="S61" s="45">
-        <v>1597</v>
+        <v>117</v>
       </c>
       <c r="T61" s="46">
-        <v>45437</v>
+        <v>45441</v>
       </c>
       <c r="U61" s="47" t="s">
-        <v>42</v>
+        <v>119</v>
       </c>
       <c r="V61" s="47"/>
       <c r="W61" s="47" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X61" s="47"/>
       <c r="Y61" s="48">
-        <v>24.34</v>
+        <v>334.43</v>
       </c>
       <c r="Z61" s="45"/>
       <c r="AA61" s="14"/>
@@ -4379,13 +4437,23 @@
       <c r="O62" s="2"/>
       <c r="P62" s="1"/>
       <c r="R62" s="45"/>
-      <c r="S62" s="45"/>
-      <c r="T62" s="46"/>
-      <c r="U62" s="47"/>
+      <c r="S62" s="45">
+        <v>118</v>
+      </c>
+      <c r="T62" s="46">
+        <v>45439</v>
+      </c>
+      <c r="U62" s="47" t="s">
+        <v>90</v>
+      </c>
       <c r="V62" s="47"/>
-      <c r="W62" s="47"/>
+      <c r="W62" s="47" t="s">
+        <v>22</v>
+      </c>
       <c r="X62" s="47"/>
-      <c r="Y62" s="48"/>
+      <c r="Y62" s="48">
+        <v>12.96</v>
+      </c>
       <c r="Z62" s="45"/>
       <c r="AA62" s="14"/>
       <c r="AB62" s="14"/>
@@ -8507,36 +8575,36 @@
     </row>
     <row r="5">
       <c r="C5" s="73" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D5" s="73" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E5" s="73">
         <v>50.4</v>
       </c>
       <c r="F5" s="73" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G5" s="73" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
       <c r="C6" s="73" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D6" s="73" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E6" s="73">
         <v>87.53</v>
       </c>
       <c r="F6" s="73" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G6" s="73" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
Additional complete items functionality
</commit_message>
<xml_diff>
--- a/TestBudget.xlsx
+++ b/TestBudget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PersonalMyCode\BudgetUpdator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C3CDDC-C703-4843-8ADD-3A888EC8B317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D38CF4-AA34-4726-9715-7168DD287CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30795" yWindow="1650" windowWidth="29010" windowHeight="15345" activeTab="2" xr2:uid="{AF956A61-A15A-4A6E-9A9E-CFD1D374AF1F}"/>
+    <workbookView xWindow="-28800" yWindow="270" windowWidth="29010" windowHeight="15345" activeTab="2" xr2:uid="{AF956A61-A15A-4A6E-9A9E-CFD1D374AF1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Income" sheetId="2" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
   <si>
     <t>May</t>
   </si>
@@ -430,6 +430,9 @@
     <t>Internet Transfer From Xxxxxxxx2900</t>
   </si>
   <si>
+    <t>asdf</t>
+  </si>
+  <si>
     <t>Donation</t>
   </si>
   <si>
@@ -437,6 +440,9 @@
   </si>
   <si>
     <t>Rocky Mountain Power</t>
+  </si>
+  <si>
+    <t>o</t>
   </si>
   <si>
     <t>ParkMobile</t>
@@ -8605,7 +8611,7 @@
   <dimension ref="A1:AR200"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8:Y47"/>
+      <selection activeCell="AC10" sqref="AC10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8764,7 +8770,7 @@
       <c r="K6" s="24"/>
       <c r="L6" s="25">
         <f>SUM(L9:L58)</f>
-        <v>0</v>
+        <v>3471.05</v>
       </c>
       <c r="M6" s="23"/>
       <c r="N6" s="23"/>
@@ -8780,7 +8786,7 @@
       <c r="X6" s="26"/>
       <c r="Y6" s="25">
         <f>SUM(Y8:Y199)</f>
-        <v>0</v>
+        <v>5410.950000000002</v>
       </c>
       <c r="Z6" s="26"/>
       <c r="AA6" s="27"/>
@@ -8957,8 +8963,14 @@
       <c r="U9" s="0" t="s">
         <v>121</v>
       </c>
+      <c r="V9" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W9" s="0" t="s">
         <v>24</v>
+      </c>
+      <c r="X9" s="0" t="s">
+        <v>122</v>
       </c>
       <c r="Y9" s="70">
         <v>-1200</v>
@@ -8999,7 +9011,7 @@
       </c>
       <c r="L10" s="42">
         <f ref="L10:L58" t="shared" si="1">SUMIF(X:X, H10, Y:Y)</f>
-        <v>0</v>
+        <v>460.96</v>
       </c>
       <c r="M10" s="42" t="e">
         <f ref="M10:M12" t="shared" si="2" ca="1">K10-L10</f>
@@ -9016,10 +9028,16 @@
         <v>45447</v>
       </c>
       <c r="U10" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
+      </c>
+      <c r="V10" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="W10" s="0" t="s">
         <v>24</v>
+      </c>
+      <c r="X10" s="0" t="s">
+        <v>122</v>
       </c>
       <c r="Y10" s="70">
         <v>1608.35</v>
@@ -9049,7 +9067,7 @@
       </c>
       <c r="D11" s="58">
         <f>Y6</f>
-        <v>0</v>
+        <v>5410.950000000002</v>
       </c>
       <c r="E11" s="40"/>
       <c r="G11" s="41"/>
@@ -9091,10 +9109,16 @@
         <v>45447</v>
       </c>
       <c r="U11" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
+      </c>
+      <c r="V11" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="W11" s="0" t="s">
         <v>24</v>
+      </c>
+      <c r="X11" s="0" t="s">
+        <v>122</v>
       </c>
       <c r="Y11" s="70">
         <v>166.81</v>
@@ -9162,10 +9186,16 @@
         <v>45447</v>
       </c>
       <c r="U12" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
+      </c>
+      <c r="V12" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="W12" s="0" t="s">
         <v>24</v>
+      </c>
+      <c r="X12" s="0" t="s">
+        <v>122</v>
       </c>
       <c r="Y12" s="70">
         <v>100</v>
@@ -9236,10 +9266,16 @@
         <v>45446</v>
       </c>
       <c r="U13" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
+      </c>
+      <c r="V13" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="W13" s="0" t="s">
         <v>24</v>
+      </c>
+      <c r="X13" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y13" s="70">
         <v>65.76</v>
@@ -9312,10 +9348,16 @@
         <v>45453</v>
       </c>
       <c r="U14" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
+      </c>
+      <c r="V14" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="W14" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X14" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y14" s="70">
         <v>12.9</v>
@@ -9346,7 +9388,7 @@
       </c>
       <c r="D15" s="60">
         <f>D9-D11</f>
-        <v>0</v>
+        <v>-5410.950000000002</v>
       </c>
       <c r="E15" s="61"/>
       <c r="F15" s="14"/>
@@ -9389,10 +9431,16 @@
         <v>45453</v>
       </c>
       <c r="U15" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
+      </c>
+      <c r="V15" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="W15" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X15" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y15" s="70">
         <v>58.51</v>
@@ -9459,8 +9507,14 @@
       <c r="U16" s="0" t="s">
         <v>97</v>
       </c>
+      <c r="V16" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W16" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X16" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y16" s="70">
         <v>186.04</v>
@@ -9528,8 +9582,14 @@
       <c r="U17" s="0" t="s">
         <v>58</v>
       </c>
+      <c r="V17" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W17" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X17" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y17" s="70">
         <v>26.74</v>
@@ -9591,8 +9651,14 @@
       <c r="U18" s="0" t="s">
         <v>58</v>
       </c>
+      <c r="V18" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W18" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X18" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y18" s="70">
         <v>25.7</v>
@@ -9652,10 +9718,16 @@
         <v>45452</v>
       </c>
       <c r="U19" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
+      </c>
+      <c r="V19" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="W19" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X19" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y19" s="70">
         <v>11.01</v>
@@ -9718,8 +9790,14 @@
       <c r="U20" s="0" t="s">
         <v>58</v>
       </c>
+      <c r="V20" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W20" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X20" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y20" s="70">
         <v>10.65</v>
@@ -9779,10 +9857,16 @@
         <v>45452</v>
       </c>
       <c r="U21" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
+      </c>
+      <c r="V21" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="W21" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X21" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y21" s="70">
         <v>65.43</v>
@@ -9833,10 +9917,16 @@
         <v>45452</v>
       </c>
       <c r="U22" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
+      </c>
+      <c r="V22" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="W22" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X22" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y22" s="70">
         <v>27.14</v>
@@ -9878,11 +9968,11 @@
       </c>
       <c r="L23" s="42">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3010.09</v>
       </c>
       <c r="M23" s="42">
         <f>K23-L23</f>
-        <v>3050</v>
+        <v>39.909999999999854</v>
       </c>
       <c r="N23" s="44"/>
       <c r="O23" s="42"/>
@@ -9954,10 +10044,16 @@
         <v>45452</v>
       </c>
       <c r="U24" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
+      </c>
+      <c r="V24" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="W24" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X24" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y24" s="70">
         <v>63.99</v>
@@ -10006,10 +10102,16 @@
         <v>45452</v>
       </c>
       <c r="U25" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
+      </c>
+      <c r="V25" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="W25" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X25" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y25" s="70">
         <v>4.28</v>
@@ -10060,8 +10162,14 @@
       <c r="U26" s="0" t="s">
         <v>58</v>
       </c>
+      <c r="V26" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W26" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X26" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y26" s="70">
         <v>40.39</v>
@@ -10112,8 +10220,14 @@
       <c r="U27" s="0" t="s">
         <v>119</v>
       </c>
+      <c r="V27" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W27" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X27" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y27" s="70">
         <v>334.43</v>
@@ -10163,10 +10277,16 @@
         <v>45450</v>
       </c>
       <c r="U28" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
+      </c>
+      <c r="V28" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="W28" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X28" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y28" s="70">
         <v>8.25</v>
@@ -10217,8 +10337,14 @@
       <c r="U29" s="0" t="s">
         <v>113</v>
       </c>
+      <c r="V29" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W29" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X29" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y29" s="70">
         <v>97.33</v>
@@ -10269,8 +10395,14 @@
       <c r="U30" s="0" t="s">
         <v>58</v>
       </c>
+      <c r="V30" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W30" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X30" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y30" s="70">
         <v>10.65</v>
@@ -10428,10 +10560,16 @@
         <v>45448</v>
       </c>
       <c r="U33" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
+      </c>
+      <c r="V33" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="W33" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X33" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y33" s="70">
         <v>10</v>
@@ -10623,8 +10761,14 @@
       <c r="U37" s="0" t="s">
         <v>58</v>
       </c>
+      <c r="V37" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W37" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X37" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y37" s="70">
         <v>105.76</v>
@@ -10673,8 +10817,14 @@
       <c r="U38" s="0" t="s">
         <v>58</v>
       </c>
+      <c r="V38" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W38" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X38" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y38" s="70">
         <v>66.31</v>
@@ -10725,8 +10875,14 @@
       <c r="U39" s="0" t="s">
         <v>58</v>
       </c>
+      <c r="V39" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W39" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X39" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y39" s="70">
         <v>17</v>
@@ -10778,8 +10934,14 @@
       <c r="U40" s="0" t="s">
         <v>95</v>
       </c>
+      <c r="V40" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W40" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X40" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y40" s="70">
         <v>24.71</v>
@@ -10828,10 +10990,16 @@
         <v>45445</v>
       </c>
       <c r="U41" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
+      </c>
+      <c r="V41" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="W41" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X41" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y41" s="70">
         <v>2</v>
@@ -11053,8 +11221,14 @@
       <c r="U45" s="0" t="s">
         <v>43</v>
       </c>
+      <c r="V45" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W45" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X45" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y45" s="70">
         <v>12.04</v>
@@ -11155,8 +11329,14 @@
       <c r="U47" s="0" t="s">
         <v>118</v>
       </c>
+      <c r="V47" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="W47" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X47" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y47" s="70">
         <v>134.84</v>
@@ -11202,10 +11382,16 @@
         <v>45454</v>
       </c>
       <c r="U48" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
+      </c>
+      <c r="V48" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="W48" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X48" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y48" s="70">
         <v>-186.04</v>
@@ -11250,10 +11436,16 @@
         <v>45454</v>
       </c>
       <c r="U49" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
+      </c>
+      <c r="V49" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="W49" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="X49" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="Y49" s="70">
         <v>28.92</v>
@@ -15839,10 +16031,10 @@
     </row>
     <row r="5">
       <c r="C5" s="73" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D5" s="73" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E5" s="73">
         <v>50.4</v>
@@ -15856,10 +16048,10 @@
     </row>
     <row r="6">
       <c r="C6" s="73" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D6" s="73" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E6" s="73">
         <v>87.53</v>

</xml_diff>